<commit_message>
TRUNG BỊ HIẾU ĐÌ NÊN PHẢI FIX BẢNG
</commit_message>
<xml_diff>
--- a/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
+++ b/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 1\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{065340E8-978B-482B-B3CA-31FDC0F3081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D804D31D-B080-42A5-9003-783FCD929083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43FC9F9E-2304-46AE-ABF6-86A58265D84E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="129">
   <si>
     <t>Test case: Trang chủ BCS</t>
   </si>
@@ -364,12 +364,6 @@
 4.F5</t>
   </si>
   <si>
-    <t>1.Di chuột đến ô đánh giá
-2.Nhập đánh giá bằng chữ
-3.Nhấn [Đánh giá]
-4.F5</t>
-  </si>
-  <si>
     <t>Nhấp vào bài viết</t>
   </si>
   <si>
@@ -379,9 +373,6 @@
     <t>Hiển thị đánh giá bao gồm tên đăng nhập và chấm điểm</t>
   </si>
   <si>
-    <t>Hiển thị tên đăng nhập và đưa ra số điểm (1-5)</t>
-  </si>
-  <si>
     <t>Trang tìm kiếm</t>
   </si>
   <si>
@@ -425,9 +416,6 @@
   </si>
   <si>
     <t>D_25</t>
-  </si>
-  <si>
-    <t>D_26</t>
   </si>
   <si>
     <t>30,m</t>
@@ -458,6 +446,33 @@
 Gmail:QUILENgmail.com
 Tên đăng nhập:meomeouser
 Mật khẩu:meomeopass </t>
+  </si>
+  <si>
+    <t>Test case: Trang ghép trọ BCS</t>
+  </si>
+  <si>
+    <t>D_26</t>
+  </si>
+  <si>
+    <t>Hiên thị thông tin trọ và giới tính người thuê trọ</t>
+  </si>
+  <si>
+    <t>D_27</t>
+  </si>
+  <si>
+    <t>Ghép trọ</t>
+  </si>
+  <si>
+    <t>1.Di chuột đến phần ghép trọ ở mỗi bài viết (Nếu có)
+2.Nhâp vào xem thông tin người ghép cùng
+3.Nhấn [Ghép cùng]
+4.Chờ đối phương xác nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiển thị thông báo nếu ghép thành công cho chủ trọ và các đối tượng muốn ghép </t>
+  </si>
+  <si>
+    <t>Trang ghép trọ</t>
   </si>
 </sst>
 </file>
@@ -569,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -611,6 +626,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,6 +646,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD530AB-72E8-4A06-B006-BA90A153AC6B}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,29 +988,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="G1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1015,7 +1045,7 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1044,7 +1074,7 @@
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1071,12 +1101,12 @@
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>33</v>
@@ -1098,7 +1128,7 @@
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
@@ -1125,7 +1155,7 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1166,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>18</v>
@@ -1152,7 +1182,7 @@
       <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="9" t="s">
         <v>28</v>
       </c>
@@ -1179,7 +1209,7 @@
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
         <v>31</v>
       </c>
@@ -1203,29 +1233,29 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="G12" s="18" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="G12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -1260,7 +1290,7 @@
       <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1283,7 +1313,7 @@
       <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="9" t="s">
         <v>46</v>
       </c>
@@ -1294,7 +1324,7 @@
         <v>48</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>18</v>
@@ -1310,7 +1340,7 @@
       <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="9" t="s">
         <v>46</v>
       </c>
@@ -1337,7 +1367,7 @@
       <c r="A18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="9" t="s">
         <v>51</v>
       </c>
@@ -1348,7 +1378,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>18</v>
@@ -1364,7 +1394,7 @@
       <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="9" t="s">
         <v>53</v>
       </c>
@@ -1388,29 +1418,29 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="G21" s="18" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="G21" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
@@ -1443,7 +1473,7 @@
     </row>
     <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>13</v>
@@ -1469,7 +1499,7 @@
     </row>
     <row r="25" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>46</v>
@@ -1495,7 +1525,7 @@
     </row>
     <row r="26" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>67</v>
@@ -1521,7 +1551,7 @@
     </row>
     <row r="27" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>69</v>
@@ -1533,7 +1563,7 @@
         <v>71</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>18</v>
@@ -1547,7 +1577,7 @@
     </row>
     <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>69</v>
@@ -1573,7 +1603,7 @@
     </row>
     <row r="29" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>73</v>
@@ -1599,7 +1629,7 @@
     </row>
     <row r="30" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>69</v>
@@ -1611,7 +1641,7 @@
         <v>77</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>18</v>
@@ -1624,29 +1654,29 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="G32" s="18" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="G32" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
@@ -1679,10 +1709,10 @@
     </row>
     <row r="35" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>102</v>
+        <v>109</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>81</v>
@@ -1694,7 +1724,7 @@
         <v>83</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>18</v>
@@ -1708,9 +1738,9 @@
     </row>
     <row r="36" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="B36" s="18"/>
       <c r="C36" s="9" t="s">
         <v>84</v>
       </c>
@@ -1735,9 +1765,9 @@
     </row>
     <row r="37" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="16"/>
+        <v>111</v>
+      </c>
+      <c r="B37" s="18"/>
       <c r="C37" s="9" t="s">
         <v>84</v>
       </c>
@@ -1762,9 +1792,9 @@
     </row>
     <row r="38" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="16"/>
+        <v>112</v>
+      </c>
+      <c r="B38" s="18"/>
       <c r="C38" s="9" t="s">
         <v>84</v>
       </c>
@@ -1788,29 +1818,29 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="G40" s="18" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="G40" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
@@ -1843,19 +1873,19 @@
     </row>
     <row r="43" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>101</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>16</v>
@@ -1872,9 +1902,9 @@
     </row>
     <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="16"/>
+        <v>114</v>
+      </c>
+      <c r="B44" s="18"/>
       <c r="C44" s="9" t="s">
         <v>95</v>
       </c>
@@ -1882,7 +1912,7 @@
         <v>96</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F44" s="9">
         <v>5</v>
@@ -1897,35 +1927,132 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="11" t="s">
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="G47" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
         <v>97</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F45" s="9">
-        <v>5</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>18</v>
+      <c r="E50" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" s="24"/>
+      <c r="C51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="23">
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="G47:I47"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="G1:I1"/>
@@ -1942,9 +2069,9 @@
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="A41:I41"/>
     <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B43:B45"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="G40:I40"/>
+    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
giao thêm cho ai ngoài trung đi chứ ko làm hết được
</commit_message>
<xml_diff>
--- a/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
+++ b/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 1\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D804D31D-B080-42A5-9003-783FCD929083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E70F5AA-5EA6-4A12-844E-A9B173C6AC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43FC9F9E-2304-46AE-ABF6-86A58265D84E}"/>
   </bookViews>
@@ -37,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
   <si>
     <t>Test case: Trang chủ BCS</t>
   </si>
   <si>
     <t>Front-end</t>
-  </si>
-  <si>
-    <t>Web</t>
   </si>
   <si>
     <t>ID</t>
@@ -92,12 +89,6 @@
   </si>
   <si>
     <t>NULL</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>Giao diện người dùng (Biểu tượng con trỏ chuột)</t>
@@ -473,6 +464,9 @@
   </si>
   <si>
     <t>Trang ghép trọ</t>
+  </si>
+  <si>
+    <t>Trang đăng nhập</t>
   </si>
 </sst>
 </file>
@@ -507,7 +501,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,12 +511,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,8 +577,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -605,9 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -632,29 +617,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD530AB-72E8-4A06-B006-BA90A153AC6B}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:I48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,1090 +974,808 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="24" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="21"/>
-      <c r="C5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>18</v>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>18</v>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="21"/>
-      <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" s="21"/>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>18</v>
+      <c r="F10" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="G12" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="A12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>18</v>
+      <c r="E17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="G21" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="A21" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>126</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>18</v>
+        <v>100</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="E28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>18</v>
+        <v>104</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>18</v>
+        <v>105</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="G32" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="A32" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
     </row>
     <row r="35" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>100</v>
+        <v>106</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>18</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="G37" s="5"/>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>18</v>
+      <c r="F38" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="G40" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
+      <c r="A40" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>101</v>
+        <v>110</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>98</v>
+        <v>12</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F44" s="9">
+      <c r="F44" s="8">
         <v>5</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="15"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>121</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="G47" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B51" s="19"/>
+      <c r="C51" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="23" t="s">
+      <c r="D51" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="E51" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>127</v>
-      </c>
       <c r="F51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A48:I48"/>
+  <mergeCells count="18">
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="A47:C47"/>
-    <mergeCell ref="G47:I47"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="G1:I1"/>
     <mergeCell ref="B4:B10"/>
-    <mergeCell ref="A22:I22"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="A33:I33"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="A13:I13"/>
     <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2090,21 +1794,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x0101005FB192C60D8CDA479E1E05FDE69506A9" ma:contentTypeVersion="4" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="86e0b5d8f6cd43469d4b0198d476de1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1e5bcc28-56d4-4657-8a9b-4429cf64ad81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddbbbd0f9bf0d1f20f4eb87448aec86e" ns3:_="">
     <xsd:import namespace="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
@@ -2248,31 +1937,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD0D57A-4EC5-4840-B0B6-C4D3306ECCDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABAC459C-3283-4A1D-9A28-344C07F57AE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2288,4 +1968,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD0D57A-4EC5-4840-B0B6-C4D3306ECCDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TRUNG MỆT LẮM RỒI
</commit_message>
<xml_diff>
--- a/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
+++ b/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 1\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE9E6B2-5637-46EF-AB4A-689D5259E23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD86A7A-129E-458A-A8B0-236EACB16C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43FC9F9E-2304-46AE-ABF6-86A58265D84E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
   <si>
     <t>Test case: Trang chủ BCS</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Kết quả</t>
-  </si>
-  <si>
-    <t>Dữ liệu/Thông số</t>
   </si>
   <si>
     <t>Chrome</t>
@@ -88,9 +85,6 @@
     <t>Hiển thị theo thiết kế có sẵn</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>Giao diện người dùng (Biểu tượng con trỏ chuột)</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
 2.Kiểm tra các bộ phận theo thiết kế có sẵn</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Các trường bắt buộc</t>
   </si>
   <si>
@@ -214,9 +205,6 @@
     <t>Hiển thị số ký tự "*" tương ứng</t>
   </si>
   <si>
-    <t>Mật khẩu: 123</t>
-  </si>
-  <si>
     <t>Test case: Trang tạo tài khoản BCS</t>
   </si>
   <si>
@@ -290,86 +278,6 @@
     <t>Test case: Trang đăng nhập BCS</t>
   </si>
   <si>
-    <t>Tên đăng nhập: Duy
-Mật khẩu: 1</t>
-  </si>
-  <si>
-    <t>Tên đăng nhập: Dũng
-Mật khẩu: 1234</t>
-  </si>
-  <si>
-    <t>Giao diện tìm kiếm</t>
-  </si>
-  <si>
-    <t>1.Ở trang chủ , di chuyển trỏ chuột vào ô nhập tìm kiếm
-2.Nhấn vào ô nhập
-3.Nhập ký tự 
-4.Nhấp tìm kiếm</t>
-  </si>
-  <si>
-    <t>Hiển thị giao diện tìm kiếm giống như thiết kế</t>
-  </si>
-  <si>
-    <t>Trường tìm kiếm</t>
-  </si>
-  <si>
-    <t>1.Không nhập gì vào ô tìm kiếm
-2. Nhấp [Tìm kiếm]</t>
-  </si>
-  <si>
-    <t>1.Nhập vào một ký tự có trong tên phim
-2.Nhấn [Tìm kiếm]</t>
-  </si>
-  <si>
-    <t>em</t>
-  </si>
-  <si>
-    <t>1.Nhập vào một ký tự 0 có trong bất kì tên phim nào
-2.Nhấn [Tìm kiếm]</t>
-  </si>
-  <si>
-    <t>***</t>
-  </si>
-  <si>
-    <t>Hiển thị toàn bộ trọ gần đây được đăng</t>
-  </si>
-  <si>
-    <t>Hiển thị các phòng trọ có tên chứa kí tự đã nhập</t>
-  </si>
-  <si>
-    <t>Không hiển thị kết quả ra</t>
-  </si>
-  <si>
-    <t>Test case: Trang tìm kiếm BCS</t>
-  </si>
-  <si>
-    <t>Test case: Trang đánh giá BCS</t>
-  </si>
-  <si>
-    <t>Trường đánh giá</t>
-  </si>
-  <si>
-    <t>1.Di chuột đến ô đánh giá
-2.Nhập đánh giá bằng số
-3.Nhấn [Đánh giá]
-4.F5</t>
-  </si>
-  <si>
-    <t>Nhấp vào bài viết</t>
-  </si>
-  <si>
-    <t>Hiển thị thông tin trọ cùng phần đánh giá giống thiết kế</t>
-  </si>
-  <si>
-    <t>Hiển thị đánh giá bao gồm tên đăng nhập và chấm điểm</t>
-  </si>
-  <si>
-    <t>Trang tìm kiếm</t>
-  </si>
-  <si>
-    <t>Trang đánh giá</t>
-  </si>
-  <si>
     <t>D_13</t>
   </si>
   <si>
@@ -389,81 +297,10 @@
   </si>
   <si>
     <t>D_19</t>
-  </si>
-  <si>
-    <t>D_20</t>
-  </si>
-  <si>
-    <t>D_21</t>
-  </si>
-  <si>
-    <t>D_22</t>
-  </si>
-  <si>
-    <t>D_23</t>
-  </si>
-  <si>
-    <t>D_24</t>
-  </si>
-  <si>
-    <t>D_25</t>
-  </si>
-  <si>
-    <t>30,m</t>
   </si>
   <si>
     <t>1.Di chuyển đến nút [Tiêu chí]
 2.Bấm [Tiêu chí]</t>
-  </si>
-  <si>
-    <t>Họ và tên: Nguyễn Trí Duy
-Ngày tháng năm sinh:01/12/2004
-SDT:02488860619
-Gmail:ONLY-CHAN@gmail.com
-Tên đăng nhập:DUY
-Mật khẩu:1</t>
-  </si>
-  <si>
-    <t>Tên đăng nhập: HiếuONLYFAN</t>
-  </si>
-  <si>
-    <t>Tên đăng nhập: Mèo Méo Mèo Meo
-Mật khẩu: 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Họ và tên: Nguyễn Quang Dũng
-Ngày tháng năm sinh:22/12/2004
-SDT:1111111111
-Gmail:QUILENgmail.com
-Tên đăng nhập:meomeouser
-Mật khẩu:meomeopass </t>
-  </si>
-  <si>
-    <t>Test case: Trang ghép trọ BCS</t>
-  </si>
-  <si>
-    <t>D_26</t>
-  </si>
-  <si>
-    <t>Hiên thị thông tin trọ và giới tính người thuê trọ</t>
-  </si>
-  <si>
-    <t>D_27</t>
-  </si>
-  <si>
-    <t>Ghép trọ</t>
-  </si>
-  <si>
-    <t>1.Di chuột đến phần ghép trọ ở mỗi bài viết (Nếu có)
-2.Nhâp vào xem thông tin người ghép cùng
-3.Nhấn [Ghép cùng]
-4.Chờ đối phương xác nhận</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiển thị thông báo nếu ghép thành công cho chủ trọ và các đối tượng muốn ghép </t>
-  </si>
-  <si>
-    <t>Trang ghép trọ</t>
   </si>
   <si>
     <t>Trang đăng nhập</t>
@@ -509,6 +346,15 @@
   </si>
   <si>
     <t>Nhận thông báo duyệt bài, hiển thị thông tin bài viết và thông tin chủ trọ, tích vào những thông tin đã kiểm duyệt và xác nhận đăng bài lên</t>
+  </si>
+  <si>
+    <t>Lỗi phát hiện ra</t>
+  </si>
+  <si>
+    <t>Chưa có</t>
+  </si>
+  <si>
+    <t>Trang bài viết</t>
   </si>
 </sst>
 </file>
@@ -614,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -650,15 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -668,29 +505,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1008,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD530AB-72E8-4A06-B006-BA90A153AC6B}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,11 +873,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1057,155 +906,155 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>9</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="9" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B6" s="21"/>
       <c r="C6" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="23"/>
+        <v>33</v>
+      </c>
+      <c r="B7" s="21"/>
       <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="B9" s="21"/>
       <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+        <v>94</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="21"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
+      <c r="A12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
@@ -1234,112 +1083,112 @@
         <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E16" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>114</v>
+      <c r="F16" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="B17" s="22"/>
       <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="E18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>117</v>
+        <v>44</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="B19" s="22"/>
       <c r="C19" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
@@ -1366,517 +1215,292 @@
         <v>6</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>126</v>
+        <v>72</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="20"/>
+        <v>73</v>
+      </c>
+      <c r="B25" s="22"/>
       <c r="C25" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="20"/>
+        <v>74</v>
+      </c>
+      <c r="B26" s="22"/>
       <c r="C26" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="20"/>
+        <v>75</v>
+      </c>
+      <c r="B27" s="22"/>
       <c r="C27" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="20"/>
+        <v>76</v>
+      </c>
+      <c r="B28" s="22"/>
       <c r="C28" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+        <v>94</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="B29" s="22"/>
       <c r="C29" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="20"/>
+        <v>78</v>
+      </c>
+      <c r="B30" s="22"/>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-    </row>
-    <row r="36" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>15</v>
+      <c r="B36" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B37" s="20"/>
-      <c r="C37" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="10" t="s">
+      <c r="C37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>84</v>
+      <c r="F37" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="G37" s="5"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B38" s="20"/>
-      <c r="C38" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>86</v>
+      <c r="C38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>110</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F44" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>119</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>121</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>127</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>135</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>138</v>
-      </c>
+      <c r="A56" s="26"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="25"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="25"/>
+      <c r="B57" s="25"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A47:C47"/>
+  <mergeCells count="13">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B4:B10"/>
-    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A48:F48"/>
     <mergeCell ref="B24:B30"/>
-    <mergeCell ref="B43:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1895,21 +1519,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x0101005FB192C60D8CDA479E1E05FDE69506A9" ma:contentTypeVersion="4" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="86e0b5d8f6cd43469d4b0198d476de1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1e5bcc28-56d4-4657-8a9b-4429cf64ad81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddbbbd0f9bf0d1f20f4eb87448aec86e" ns3:_="">
     <xsd:import namespace="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
@@ -2053,31 +1662,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD0D57A-4EC5-4840-B0B6-C4D3306ECCDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABAC459C-3283-4A1D-9A28-344C07F57AE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2093,4 +1693,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD0D57A-4EC5-4840-B0B6-C4D3306ECCDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>